<commit_message>
New calculcation for the annotation check added
</commit_message>
<xml_diff>
--- a/Datasets/Annotated/Polarity Check Results/Polarity Check Calculation.xlsx
+++ b/Datasets/Annotated/Polarity Check Results/Polarity Check Calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Annotated\Polarity Check Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vuobe\github\bachelorthesis\Datasets\Annotated\Polarity Check Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC04DFC-1B7B-481D-BBA7-59BACC013691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437DCC2E-0FD4-4EC5-8432-3022E076B591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3135" windowWidth="24240" windowHeight="17640" xr2:uid="{68571775-85D3-4795-B5CD-656936DFB7F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{68571775-85D3-4795-B5CD-656936DFB7F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1199,7 +1199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1215,7 +1215,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1514,10 +1514,10 @@
   <dimension ref="A1:R266"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
@@ -1653,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:L66" si="2">(1/(4*(4-1))*(J3^2+K3^2-4))</f>
+        <f>((1/(4*(4-1)))*(J3^2+K3^2-4))</f>
         <v>0.5</v>
       </c>
       <c r="N3" t="s">
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L3:L66" si="2">(1/(4*(4-1))*(J4^2+K4^2-4))</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>